<commit_message>
updated performance file 2
</commit_message>
<xml_diff>
--- a/performance2.xlsx
+++ b/performance2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\3244\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mintee/Desktop/3244/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBE45DE-2681-4AC3-BEB3-78A612F8662E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14377D5A-9C30-2D40-9079-8C20E005AC2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3756" yWindow="2400" windowWidth="30960" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17520" windowHeight="14600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="94">
   <si>
     <t>Features</t>
   </si>
@@ -232,6 +232,81 @@
   </si>
   <si>
     <t>high result variation</t>
+  </si>
+  <si>
+    <t>DT</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>0.62/0.62</t>
+  </si>
+  <si>
+    <t>0.59/0.59</t>
+  </si>
+  <si>
+    <t>0.43/0.42</t>
+  </si>
+  <si>
+    <t>0.42/0.43</t>
+  </si>
+  <si>
+    <t>0.19/0.19</t>
+  </si>
+  <si>
+    <t>0.16/0.16</t>
+  </si>
+  <si>
+    <t>0.19/0.18</t>
+  </si>
+  <si>
+    <t>0.52/0.48</t>
+  </si>
+  <si>
+    <t>0.49/0.45</t>
+  </si>
+  <si>
+    <t>0.54/0.50</t>
+  </si>
+  <si>
+    <t>0.26/0.22</t>
+  </si>
+  <si>
+    <t>0.23/0.19</t>
+  </si>
+  <si>
+    <t>0.25/0.21</t>
+  </si>
+  <si>
+    <t>0.65/0.64</t>
+  </si>
+  <si>
+    <t>0.52/0.50</t>
+  </si>
+  <si>
+    <t>0.51/0.48</t>
+  </si>
+  <si>
+    <t>0.49/0.46</t>
+  </si>
+  <si>
+    <t>0.67/0.66</t>
+  </si>
+  <si>
+    <t>0.40/0.40</t>
+  </si>
+  <si>
+    <t>0.44/0.43</t>
+  </si>
+  <si>
+    <t>0.25/0.22</t>
+  </si>
+  <si>
+    <t>0.24/0.21</t>
+  </si>
+  <si>
+    <t>0.26/0.23</t>
   </si>
 </sst>
 </file>
@@ -573,26 +648,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.109375" customWidth="1"/>
-    <col min="2" max="2" width="33.77734375" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="33.83203125" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
     <col min="8" max="8" width="19.6640625" customWidth="1"/>
-    <col min="9" max="9" width="27.21875" customWidth="1"/>
+    <col min="9" max="9" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -621,7 +696,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -650,7 +725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -679,7 +754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -705,70 +780,61 @@
         <v>0.70660000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.61660000000000004</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.61660000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F6" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="G6" s="2">
-        <v>0.72660000000000002</v>
+        <v>0.70330000000000004</v>
       </c>
       <c r="H6" s="2">
-        <v>0.71660000000000001</v>
-      </c>
-      <c r="I6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0.67</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0.67</v>
-      </c>
-      <c r="I7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -777,367 +843,688 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.72660000000000002</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.71660000000000001</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>29</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E10" t="s">
         <v>66</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F10" t="s">
         <v>67</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G10" s="2">
         <v>0.68659999999999999</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H10" s="2">
         <v>0.69</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0.52659999999999996</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0.45329999999999998</v>
-      </c>
-      <c r="I10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="G11" s="2">
-        <v>0.45</v>
+        <v>0.63</v>
       </c>
       <c r="H11" s="2">
-        <v>0.45</v>
-      </c>
-      <c r="I11" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.62660000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="G12" s="2">
-        <v>0.50660000000000005</v>
+        <v>0.67</v>
       </c>
       <c r="H12" s="2">
-        <v>0.49</v>
-      </c>
-      <c r="J12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.6633</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>17</v>
+      <c r="B14" t="s">
+        <v>16</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="G14" s="2">
-        <v>0.56000000000000005</v>
+        <v>0.52659999999999996</v>
       </c>
       <c r="H14" s="2">
-        <v>0.4733</v>
+        <v>0.45329999999999998</v>
       </c>
       <c r="I14" t="s">
         <v>11</v>
       </c>
       <c r="J14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="G15" s="2">
-        <v>0.46329999999999999</v>
+        <v>0.45</v>
       </c>
       <c r="H15" s="2">
-        <v>0.46329999999999999</v>
+        <v>0.45</v>
       </c>
       <c r="I15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="G16" s="2">
-        <v>0.49330000000000002</v>
+        <v>0.50660000000000005</v>
       </c>
       <c r="H16" s="2">
-        <v>0.47660000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.49</v>
+      </c>
+      <c r="J16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="F18" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="G18" s="2">
-        <v>0.27</v>
+        <v>0.51659999999999995</v>
       </c>
       <c r="H18" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="I18" t="s">
+        <v>0.47660000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.4733</v>
+      </c>
+      <c r="I20" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="J20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" t="s">
-        <v>44</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0.1966</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0.18659999999999999</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.46329999999999999</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.46329999999999999</v>
+      </c>
+      <c r="I21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>12</v>
       </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="2">
-        <v>0.18659999999999999</v>
-      </c>
-      <c r="H20" s="2">
-        <v>0.1933</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" t="s">
         <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G22" s="2">
-        <v>0.2666</v>
+        <v>0.49330000000000002</v>
       </c>
       <c r="H22" s="2">
-        <v>0.1633</v>
-      </c>
-      <c r="I22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.47660000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="F23" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="G23" s="2">
-        <v>0.2233</v>
+        <v>0.42330000000000001</v>
       </c>
       <c r="H23" s="2">
-        <v>0.21329999999999999</v>
-      </c>
-      <c r="I23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.41660000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
         <v>17</v>
       </c>
       <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.50660000000000005</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
         <v>7</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="I26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.1966</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0.18659999999999999</v>
+      </c>
+      <c r="I27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.18659999999999999</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0.1933</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" t="s">
+        <v>77</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.17660000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" t="s">
+        <v>83</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.24660000000000001</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0.20660000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" t="s">
+        <v>57</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.2666</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0.1633</v>
+      </c>
+      <c r="I32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" t="s">
+        <v>44</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.2233</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0.21329999999999999</v>
+      </c>
+      <c r="I33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
         <v>60</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E34" t="s">
         <v>60</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F34" t="s">
         <v>60</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G34" s="2">
         <v>0.15</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H34" s="2">
         <v>0.16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" t="s">
+        <v>77</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0.19329999999999997</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0.18659999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" t="s">
+        <v>92</v>
+      </c>
+      <c r="F36" t="s">
+        <v>93</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>